<commit_message>
downloaded notebooks and forks
</commit_message>
<xml_diff>
--- a/notebooks/notebooks_info.xlsx
+++ b/notebooks/notebooks_info.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jimmy\Documents\GitHub\KGTorrent\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6560DD10-F1B3-456F-B505-1A27511E8C4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CEB2E6B-E054-4B66-9D6B-D993F7DD402E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27915" yWindow="5955" windowWidth="28035" windowHeight="14790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29475" yWindow="75" windowWidth="25995" windowHeight="8475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
   <si>
     <t>UserName</t>
   </si>
@@ -151,13 +152,85 @@
   </si>
   <si>
     <t>cracking-the-walmart-sales-forecasting-challenge</t>
+  </si>
+  <si>
+    <t>Nbconvert encoding support limited</t>
+  </si>
+  <si>
+    <t>Add documentation</t>
+  </si>
+  <si>
+    <t>Forked code</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Append model training code to data processing code (may benefit from forking tool due to the need for trial and error during training).</t>
+  </si>
+  <si>
+    <t>Data processing and splitting</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Simple ML model with data processing</t>
+  </si>
+  <si>
+    <t>Idea: forking between notebooks and smart merge or merge based on user defined cells, benefits original code</t>
+  </si>
+  <si>
+    <t>New features (e.g., GPU support), model changes, different model types (may benefit from forking), different loss functions (may benefit from forking)</t>
+  </si>
+  <si>
+    <t>Idea 2: fork from multiple sources (pick and choose)</t>
+  </si>
+  <si>
+    <t>Parameter changes, different model type, changes to data processing (due to the different model)</t>
+  </si>
+  <si>
+    <t>Different weights, added a model to the starter notebook which only contained data processing, added data processing for training data and validation data</t>
+  </si>
+  <si>
+    <t>Adapted original notebook to add enhanced data processing. Original notebook served as a baseline for basic usage of a tool. Original data did not change</t>
+  </si>
+  <si>
+    <t>Tool usage template</t>
+  </si>
+  <si>
+    <t>Q: how to fix this? A lot repeated code, but also a lot that is different</t>
+  </si>
+  <si>
+    <t>Model evaluation and comparison (from model files); data processing</t>
+  </si>
+  <si>
+    <t>Added plotting of results, changed most of the data processing, Adapted original notebook for inference problem using a model file instead of training and model accuracy evaluation of a set of models. Author has made other notebooks which fork from same origin as this one.</t>
+  </si>
+  <si>
+    <t>Data processing and exploration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Starts diverging after the 5th cell (forking could be useful); added train test split; data sampling is slightly different; replace data visualization and data output portions with model training - added model training, model selection, model evaluation; </t>
+  </si>
+  <si>
+    <t>Removed some feature engineering code, different plots in some cases, small changes to the way relations between variables are displayed. Model training section did not change</t>
+  </si>
+  <si>
+    <t>small variable and parameter changes during data processing; large changes in the model. This notebook was used for an alternative exploration; can incorporate forking</t>
+  </si>
+  <si>
+    <t>Removed and added import statements; added additional functions; code is different everywhere except for the majority of the import statements</t>
+  </si>
+  <si>
+    <t>Demonstration of a library</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +242,14 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -203,17 +284,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -513,16 +600,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
     <col min="5" max="5" width="47.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -550,8 +637,8 @@
       <c r="D2">
         <v>3670308</v>
       </c>
-      <c r="E2" t="str">
-        <f>CONCATENATE("https://www.kaggle.com/",B2,"/",C2)</f>
+      <c r="E2" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.kaggle.com/",B2,"/",C2))</f>
         <v>https://www.kaggle.com/annavictoria/ml-friendly-public-datasets</v>
       </c>
     </row>
@@ -568,8 +655,8 @@
       <c r="D3">
         <v>37607473</v>
       </c>
-      <c r="E3" t="str">
-        <f t="shared" ref="E3:E21" si="0">CONCATENATE("https://www.kaggle.com/",B3,"/",C3)</f>
+      <c r="E3" s="2" t="str">
+        <f t="shared" ref="E3:E21" si="0">HYPERLINK(CONCATENATE("https://www.kaggle.com/",B3,"/",C3))</f>
         <v>https://www.kaggle.com/nvnnghia/yolov5-pseudo-labeling</v>
       </c>
     </row>
@@ -586,7 +673,7 @@
       <c r="D4">
         <v>43165237</v>
       </c>
-      <c r="E4" t="str">
+      <c r="E4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>https://www.kaggle.com/its7171/gru-lstm-with-feature-engineering-and-augmentation</v>
       </c>
@@ -604,7 +691,7 @@
       <c r="D5">
         <v>1683906</v>
       </c>
-      <c r="E5" t="str">
+      <c r="E5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>https://www.kaggle.com/aharless/xgboost-cv-lb-284</v>
       </c>
@@ -622,7 +709,7 @@
       <c r="D6">
         <v>33624889</v>
       </c>
-      <c r="E6" t="str">
+      <c r="E6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>https://www.kaggle.com/nvnnghia/fasterrcnn-pseudo-labeling</v>
       </c>
@@ -640,7 +727,7 @@
       <c r="D7">
         <v>43198782</v>
       </c>
-      <c r="E7" t="str">
+      <c r="E7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>https://www.kaggle.com/its7171/how-to-generate-augmentation-data</v>
       </c>
@@ -658,7 +745,7 @@
       <c r="D8">
         <v>34656263</v>
       </c>
-      <c r="E8" t="str">
+      <c r="E8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>https://www.kaggle.com/shonenkov/oof-evaluation-mixup-efficientdet</v>
       </c>
@@ -676,7 +763,7 @@
       <c r="D9">
         <v>2229114</v>
       </c>
-      <c r="E9" t="str">
+      <c r="E9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>https://www.kaggle.com/kmader/train-simple-xray-cnn</v>
       </c>
@@ -694,7 +781,7 @@
       <c r="D10">
         <v>3746212</v>
       </c>
-      <c r="E10" t="str">
+      <c r="E10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>https://www.kaggle.com/osciiart/homecreditrisk-extensive-eda-baseline-model-jp</v>
       </c>
@@ -712,7 +799,7 @@
       <c r="D11">
         <v>3164183</v>
       </c>
-      <c r="E11" t="str">
+      <c r="E11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>https://www.kaggle.com/kmader/attention-on-pretrained-vgg16-for-bone-age</v>
       </c>
@@ -730,7 +817,7 @@
       <c r="D12">
         <v>42199959</v>
       </c>
-      <c r="E12" t="str">
+      <c r="E12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>https://www.kaggle.com/corochann/lyft-deep-into-the-l5kit-library</v>
       </c>
@@ -748,7 +835,7 @@
       <c r="D13">
         <v>44561351</v>
       </c>
-      <c r="E13" t="str">
+      <c r="E13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>https://www.kaggle.com/kushal1506/moa-pytorch-0-01859-rankgauss-pca-nn</v>
       </c>
@@ -766,7 +853,7 @@
       <c r="D14">
         <v>1920358</v>
       </c>
-      <c r="E14" t="str">
+      <c r="E14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>https://www.kaggle.com/aeryan/spotify-music-analysis</v>
       </c>
@@ -784,7 +871,7 @@
       <c r="D15">
         <v>38064567</v>
       </c>
-      <c r="E15" t="str">
+      <c r="E15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>https://www.kaggle.com/whurobin/wbf-over-tta-single-model-fasterrcnn-resnest</v>
       </c>
@@ -802,7 +889,7 @@
       <c r="D16">
         <v>3118790</v>
       </c>
-      <c r="E16" t="str">
+      <c r="E16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>https://www.kaggle.com/rhodiumbeng/classifying-multi-label-comments-0-9741-lb</v>
       </c>
@@ -820,7 +907,7 @@
       <c r="D17">
         <v>38912000</v>
       </c>
-      <c r="E17" t="str">
+      <c r="E17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>https://www.kaggle.com/amyjang/tensorflow-transfer-learning-melanoma</v>
       </c>
@@ -838,7 +925,7 @@
       <c r="D18">
         <v>43842728</v>
       </c>
-      <c r="E18" t="str">
+      <c r="E18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>https://www.kaggle.com/sx2154/gfootball-rules-from-environment-exploration</v>
       </c>
@@ -856,7 +943,7 @@
       <c r="D19">
         <v>42679125</v>
       </c>
-      <c r="E19" t="str">
+      <c r="E19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>https://www.kaggle.com/gogo827jz/moa-lstm-pure-transformer-fast-and-not-bad</v>
       </c>
@@ -874,7 +961,7 @@
       <c r="D20">
         <v>39296252</v>
       </c>
-      <c r="E20" t="str">
+      <c r="E20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>https://www.kaggle.com/raininbox/train-efficientdet-like-yolo-v5</v>
       </c>
@@ -892,12 +979,242 @@
       <c r="D21">
         <v>3025467</v>
       </c>
-      <c r="E21" t="str">
+      <c r="E21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>https://www.kaggle.com/fernandol/cracking-the-walmart-sales-forecasting-challenge</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A39BF35-C635-4263-8804-29D74E63CA8B}">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="94.5703125" customWidth="1"/>
+    <col min="3" max="3" width="72.28515625" customWidth="1"/>
+    <col min="4" max="4" width="51.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changed num_notebooks to num_repos
variable name makes more sense
</commit_message>
<xml_diff>
--- a/notebooks/notebooks_info.xlsx
+++ b/notebooks/notebooks_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jimmy\Documents\GitHub\KGTorrent\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CEB2E6B-E054-4B66-9D6B-D993F7DD402E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C8D325-2269-4447-B196-F73827529AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29475" yWindow="75" windowWidth="25995" windowHeight="8475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="76">
   <si>
     <t>UserName</t>
   </si>
@@ -224,13 +224,51 @@
   </si>
   <si>
     <t>Demonstration of a library</t>
+  </si>
+  <si>
+    <t>ML model with data processing</t>
+  </si>
+  <si>
+    <t>Changed NN architecture, removed some layers and changed dropout; changed input data path
+Purpose was to build a better model than the forked baseline; could benefit from forking and version control</t>
+  </si>
+  <si>
+    <t>Data analysis and plotting</t>
+  </si>
+  <si>
+    <t>Practically unchanged; removed some comments</t>
+  </si>
+  <si>
+    <t>Hyperparameters different; Model changed, however the bulk of the data processing, model prediction and plotting is virtually unchanged. Some data processing parameters changed</t>
+  </si>
+  <si>
+    <t>Almost no similarity between the two files aside from some standard import statements and some model fitting lines</t>
+  </si>
+  <si>
+    <t>Code template/skeleton</t>
+  </si>
+  <si>
+    <t>Finished code with data processing and model training (divergence after In[3])</t>
+  </si>
+  <si>
+    <t>Improvement on original model; Divergence begins at In[9] -&gt; changes to image processing function (although 5 more cells afterwards are identical)
+changes to learning rate optimization</t>
+  </si>
+  <si>
+    <t>Loss function changed, model changed (model copied from another source); minor changes in the import statements</t>
+  </si>
+  <si>
+    <t>Hyperparameter changes, model fitting changes (minor changes); added mixed_precision and gradient accumulation; no changes to data processing</t>
+  </si>
+  <si>
+    <t>significant changes and additions to data processing; changed model. Kept code for submission, file reading</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,13 +289,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -284,11 +335,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -297,8 +349,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="差" xfId="2" builtinId="27"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
@@ -603,17 +659,18 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="19.140625" customWidth="1"/>
     <col min="5" max="5" width="47.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -624,7 +681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -642,7 +699,7 @@
         <v>https://www.kaggle.com/annavictoria/ml-friendly-public-datasets</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -660,7 +717,7 @@
         <v>https://www.kaggle.com/nvnnghia/yolov5-pseudo-labeling</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -678,7 +735,7 @@
         <v>https://www.kaggle.com/its7171/gru-lstm-with-feature-engineering-and-augmentation</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -696,7 +753,7 @@
         <v>https://www.kaggle.com/aharless/xgboost-cv-lb-284</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -714,7 +771,7 @@
         <v>https://www.kaggle.com/nvnnghia/fasterrcnn-pseudo-labeling</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -732,7 +789,7 @@
         <v>https://www.kaggle.com/its7171/how-to-generate-augmentation-data</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -750,7 +807,7 @@
         <v>https://www.kaggle.com/shonenkov/oof-evaluation-mixup-efficientdet</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -768,7 +825,7 @@
         <v>https://www.kaggle.com/kmader/train-simple-xray-cnn</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -786,7 +843,7 @@
         <v>https://www.kaggle.com/osciiart/homecreditrisk-extensive-eda-baseline-model-jp</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -804,7 +861,7 @@
         <v>https://www.kaggle.com/kmader/attention-on-pretrained-vgg16-for-bone-age</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -822,7 +879,7 @@
         <v>https://www.kaggle.com/corochann/lyft-deep-into-the-l5kit-library</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -840,7 +897,7 @@
         <v>https://www.kaggle.com/kushal1506/moa-pytorch-0-01859-rankgauss-pca-nn</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -858,7 +915,7 @@
         <v>https://www.kaggle.com/aeryan/spotify-music-analysis</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -876,7 +933,7 @@
         <v>https://www.kaggle.com/whurobin/wbf-over-tta-single-model-fasterrcnn-resnest</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -894,7 +951,7 @@
         <v>https://www.kaggle.com/rhodiumbeng/classifying-multi-label-comments-0-9741-lb</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -912,7 +969,7 @@
         <v>https://www.kaggle.com/amyjang/tensorflow-transfer-learning-melanoma</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -930,7 +987,7 @@
         <v>https://www.kaggle.com/sx2154/gfootball-rules-from-environment-exploration</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -948,7 +1005,7 @@
         <v>https://www.kaggle.com/gogo827jz/moa-lstm-pure-transformer-fast-and-not-bad</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -966,7 +1023,7 @@
         <v>https://www.kaggle.com/raininbox/train-efficientdet-like-yolo-v5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -984,7 +1041,7 @@
         <v>https://www.kaggle.com/fernandol/cracking-the-walmart-sales-forecasting-challenge</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="B23" t="s">
         <v>40</v>
       </c>
@@ -998,18 +1055,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A39BF35-C635-4263-8804-29D74E63CA8B}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="94.5703125" customWidth="1"/>
     <col min="3" max="3" width="72.28515625" customWidth="1"/>
     <col min="4" max="4" width="51.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" t="s">
         <v>42</v>
       </c>
@@ -1017,7 +1074,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1028,7 +1085,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="30">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1039,7 +1096,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="30">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1050,7 +1107,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="30">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1061,7 +1118,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="45">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1072,7 +1129,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="45">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1083,7 +1140,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="60">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1097,7 +1154,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="60">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1108,7 +1165,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="45">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1119,7 +1176,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="45">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1130,7 +1187,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="30">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1141,75 +1198,111 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="60">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="45">
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30">
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30">
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30">
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30">
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="B25" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="B26" t="s">
         <v>50</v>
       </c>

</xml_diff>